<commit_message>
feat: update calculation ragas
</commit_message>
<xml_diff>
--- a/test/human/data/data_testcase.xlsx
+++ b/test/human/data/data_testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\human\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A99BDB-369B-415C-BDC0-7B30C0FE5D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E46AA-4662-4651-ADA2-9DA644DEDA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7FD8239-2D96-4688-A048-ADBE3AAB3502}"/>
   </bookViews>
@@ -545,23 +545,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,12 +577,31 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -603,7 +620,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -622,7 +639,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -636,31 +653,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -676,12 +674,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DE5294B-EEB2-4C8B-A347-1013CA7914CB}" name="Table13" displayName="Table13" ref="A1:C51" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DE5294B-EEB2-4C8B-A347-1013CA7914CB}" name="Table13" displayName="Table13" ref="A1:C51" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:C51" xr:uid="{CA3EBB52-0541-4D84-AA27-B220DF286A8D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B3B35749-B31A-4D58-B0DB-CB4B8BEB47E8}" name="No" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{850681BF-3655-4370-B3FA-48A29C2D0164}" name="Question" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{FC230C4E-D812-43B5-9246-5219C076560C}" name="Ground Truth" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B3B35749-B31A-4D58-B0DB-CB4B8BEB47E8}" name="No" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{850681BF-3655-4370-B3FA-48A29C2D0164}" name="Question" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FC230C4E-D812-43B5-9246-5219C076560C}" name="Ground Truth" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -987,575 +985,575 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="176" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="59.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="226.5703125" style="5" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="5" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="165" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="285" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="105" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="120" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="150" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="105" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="180" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="165" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="165" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="120" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="165" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="5" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update ragas calculation critical
</commit_message>
<xml_diff>
--- a/test/human/data/data_testcase.xlsx
+++ b/test/human/data/data_testcase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Features\Documents\PMB-UNDIKSHA\va-pmb-undiksha\test\human\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PMB-UNDIKSHA\va-pmb-undiksha\test\human\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281E46AA-4662-4651-ADA2-9DA644DEDA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFB12F6-2F87-4329-9483-8830416CC7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7FD8239-2D96-4688-A048-ADBE3AAB3502}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Saya ingin tahu terkait dengan Beasiswa Afirmasi Dikti (Adik) Papua</t>
   </si>
@@ -51,21 +51,6 @@
     <t>Berikan informasi tentang Fakultas Bahasa dan Seni</t>
   </si>
   <si>
-    <t>Saya ingin cek kelulusan SMBJM nomor pendaftaran 3242000006 tanggal lahir 2005-11-30</t>
-  </si>
-  <si>
-    <t>Saya bingung mau lihat status kelulusan SMBJM</t>
-  </si>
-  <si>
-    <t>Dimana saya bisa melihat KTM?</t>
-  </si>
-  <si>
-    <t>Kapan program studi Pendidikan Olahraga dan Kesehatan pertama kali berdiri di bawah Jurusan Pendidikan Matematika dan Ilmu Pengetahuan Alam (MIPA)?</t>
-  </si>
-  <si>
-    <t>Apa saja jenis kecerdasan yang dikembangkan dalam kurikulum Undiksha berdasarkan falsafah Tri Hita Karana?</t>
-  </si>
-  <si>
     <t>Di mana informasi lebih lanjut mengenai prosedur pembayaran UKT dengan BRIVA dapat ditemukan?</t>
   </si>
   <si>
@@ -84,9 +69,6 @@
     <t>Apa saja kriteria peserta UTBK?</t>
   </si>
   <si>
-    <t>Apa prinsip SNPMB?</t>
-  </si>
-  <si>
     <t>Kapan jadwal SNBP?</t>
   </si>
   <si>
@@ -108,12 +90,6 @@
     <t>Pengembangan kurikulum Undiksha sesuai dengan apa?</t>
   </si>
   <si>
-    <t>Siapa nama Direktur Pascasarjana Universitas Pendidikan Ganesha?</t>
-  </si>
-  <si>
-    <t>Sebutkan program doktoral yang ditawarkan oleh Fakultas Pascasarjana Universitas Pendidikan Ganesha.</t>
-  </si>
-  <si>
     <t>Bagaimana cara mendapat informasi lebih lanjut tentang UKM di Undiksha?</t>
   </si>
   <si>
@@ -123,67 +99,16 @@
     <t>FHIS punya video profil?</t>
   </si>
   <si>
-    <t>Coba kirimkan web FHIS</t>
-  </si>
-  <si>
     <t>Apa itu Estimasi Biaya Kuliah?</t>
   </si>
   <si>
-    <t>Visi Fakultas Ekonomi</t>
-  </si>
-  <si>
     <t>Kapan jadwal pendaftaran SMBJM?</t>
   </si>
   <si>
-    <t>Siapa nama Wakil Dekan I FE?</t>
-  </si>
-  <si>
-    <t>Siapa nama Dekan FIP?</t>
-  </si>
-  <si>
-    <t>Kapan FIP mulai berdiri dan apa jurusan awalnya?</t>
-  </si>
-  <si>
-    <t>Link informasi cara pembayaran UKT Mahasiswa Baru Undiksha dengan Layanan BRI Virtual Account (BRIVA)</t>
-  </si>
-  <si>
-    <t>Saya ingin lihat KTM, NIM saya 2115101014.</t>
-  </si>
-  <si>
-    <t>Siapa presiden indonesia sekarang?</t>
-  </si>
-  <si>
     <t>Berapa daya tampung mahasiswa program studi ilmu komputer S1?</t>
   </si>
   <si>
-    <t>Kapan FK didirikan?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FK?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FMIPA?</t>
-  </si>
-  <si>
-    <t>Siapa Dekan FMIPA?</t>
-  </si>
-  <si>
-    <t>Apa visi dari FOK?</t>
-  </si>
-  <si>
-    <t>Kapan FTK mulai berdiri dan program studi awal apa yang ditawarkan?</t>
-  </si>
-  <si>
-    <t>Siapa Dekan FTK?</t>
-  </si>
-  <si>
     <t>Apa fungsi utama UKM di Universitas Pendidikan Ganesha?</t>
-  </si>
-  <si>
-    <t>Apa tugas utama dari UPA TIK?</t>
-  </si>
-  <si>
-    <t>Siapa kepala UPA TIK saat ini?</t>
   </si>
   <si>
     <t>Ground Truth</t>
@@ -269,86 +194,11 @@
   </si>
   <si>
     <t>Salam Harmoni🙏
-Nama Wakil Dekan I Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah Dr. Dra. Ni Made Suci, M.Si.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Ekonomi (FE) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Berjiwa Wirausaha Berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045."</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat mengunjungi website Fakultas Hukum dan Ilmu Sosial Universitas Pendidikan Ganesha (Undiksha) melalui tautan berikut: http://fhis.undiksha.ac.id</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
 Ya, Fakultas Hukum dan Ilmu Sosial (FHIS) Universitas Pendidikan Ganesha memiliki video profil. Anda dapat menontonnya melalui tautan berikut: https://youtu.be/xrruGWs5HNk. Video ini memberikan informasi mengenai program studi, kegiatan, dan keunggulan yang ditawarkan oleh FHIS</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
-Nama dekan Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha adalah Prof. Dr. I Wayan Widiana, S.Pd., M.Pd.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Ilmu Pendidikan (FIP) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1968. Jurusan awal yang ada di fakultas ini adalah Bimbingan dan Penyuluhan serta Pendidikan Luar Sekolah.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Kedokteran Universitas Pendidikan Ganesha (Undiksha) didirikan berdasarkan Keputusan Menteri Riset Teknologi dan Pendidikan Tinggi Republik Indonesia, Nomor: 574/KPT/I/2018 tertanggal 16 Juli 2018.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Kedokteran (FK) Universitas Pendidikan Ganesha adalah menjadi program studi kedokteran unggul dalam bidang kedokteran pariwisata berlandaskan Falsafah Tri Hita Karana di Asia Tahun 2045.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah "Menjadi Fakultas Unggul Dalam Matematika Dan Ilmu Pengetahuan Alam Berlandaskan Falsafah Tri Hita Karana Di Asia Tahun 2045."</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Dekan Fakultas Matematika dan Ilmu Pengetahuan Alam (FMIPA) Universitas Pendidikan Ganesha adalah Dr. I Wayan Sukra Warpala, S.Pd., M.Sc.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Program Studi Pendidikan Olahraga dan Kesehatan pertama kali berdiri pada tahun 1988 di bawah Jurusan Pendidikan Matematika dan Ilmu Pengetahuan Alam (MIPA).</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Visi Fakultas Olahraga dan Kesehatan (FOK) Universitas Pendidikan Ganesha adalah menjadi Fakultas unggul dalam menghasilkan Sumber Daya Manusia (SDM) di bidang keolahragaan dan kesehatan berlandaskan falsafah Tri Hita Karana di Indonesia tahun 2045.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha mulai berdiri pada tahun 1990. Program studi awal yang ditawarkan adalah Pendidikan Kesejahteraan Keluarga di bawah Jurusan Ilmu Pendidikan.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Dekan Fakultas Teknik dan Kejuruan (FTK) Universitas Pendidikan Ganesha adalah Dr. Kadek Rihendra Dantes, S.T., M.T.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
 Kurikulum dikembangkan sesuai dengan visi, misi, tujuan, dan sasaran Undiksha yang berbasis kompetensi dan berorientasi Kerangka Kualifikasi Nasional Indonesia (KKNI).</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-1. Kecerdasan Intelektual: Pengembangan kemampuan berpikir kritis, analitis, dan kreatif.
-2. Kecerdasan Spiritual: Harmonisasi hubungan civitas akademika dengan Sang Pencipta.
-3. Kecerdasan Sosial: Harmonisasi hubungan antar sesama civitas akademika.
-4. Kecerdasan Ekologis: Harmonisasi hubungan civitas akademika dengan lingkungan.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Direktur Pascasarjana Universitas Pendidikan Ganesha adalah Prof. Dr. I Nyoman Jampel, M.Pd.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-1. Doktor Pendidikan Dasar
-2. Doktor Ilmu Pendidikan
-3. Doktor Pendidikan Bahasa
-4. Doktor Pendidikan Bahasa Inggris
-5. Doktor Teknologi Pendidikan</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat mengakses informasi mengenai tata cara pembayaran Uang Kuliah Tunggal (UKT) mahasiswa baru Universitas Pendidikan Ganesha dengan layanan BRI Virtual Account (BRIVA) melalui link berikut: https://undiksha.ac.id/prosedur-pembayaran-ukt-mahasiswa-baru-undiksha-dengan-layanan-bri-virtual-account-briva</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -358,15 +208,6 @@
     <t>Salam Harmoni🙏
 1. Lulusan SMA/SMK/MA/Sederajat tahun 2023, 2024, dan 2025.
 2. Lulusan Paket C tahun 2023, 2024, dan 2025 dengan umur maksimal 25 tahun (per 1 Juli 2025).</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-1. Fleksibel: Proses seleksi dirancang untuk memberikan kemudahan bagi peserta dalam mengikuti ujian.
-2. Efisien: Mengutamakan penggunaan sumber daya secara optimal untuk mencapai hasil yang maksimal.
-3. Transparan: Proses seleksi dilakukan secara terbuka dan dapat dipertanggungjawabkan.
-4. Adil: Memberikan kesempatan yang sama bagi semua peserta tanpa diskriminasi.
-5. Larangan Berkonflik: Menghindari adanya konflik kepentingan dalam proses seleksi.
-6. Akuntabel: Setiap tahapan dan keputusan dalam proses seleksi dapat dipertanggungjawabkan.</t>
   </si>
   <si>
     <t>Salam Harmoni🙏
@@ -417,22 +258,6 @@
   </si>
   <si>
     <t>Salam Harmoni🙏
-Tugas utama dari UPA TIK Universitas Pendidikan Ganesha adalah melaksanakan pengembangan, pengelolaan, dan pelayanan teknologi informasi dan komunikasi serta pengelolaan sistem informasi dan jaringan. Secara lebih rinci, UPA TIK menyelenggarakan beberapa fungsi, yaitu:
-1. Penyusunan rencana, program, dan anggaran UPA.
-2. Pengembangan teknologi informasi dan komunik.
-3. Pengelolaan teknologi informasi dan komunikasi.
-4. Pemberian layanan di bidang teknologi informasi dan komunikasi.
-5. Pengembangan dan pengelolaan sistem informasi.
-6. Pengembangan dan pengelolaan jaringan.
-7. Pemeliharaan dan perbaikan jaringan.
-8. Pelaksanaan urusan tata usaha UPA.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Kepala UPA TIK Universitas Pendidikan Ganesha saat ini adalah I Ketut Resika Arthana, S.T., M.Kom.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
 Motto Universitas Pendidikan Ganesha (Undiksha) adalah “dharmaning sajjana umerdhyaken widyaguna” yang berarti kewajiban orang bijaksana adalah mengembangkan ilmu pengetahuan dan pekerti.</t>
   </si>
   <si>
@@ -449,44 +274,7 @@
 Rektor Universitas Pendidikan Ganesha saat ini adalah Prof. Dr. I Wayan Lasmawan, M.Pd.</t>
   </si>
   <si>
-    <t>Salam Harmoni🙏
-Berikut informasi Kelulusan Peserta SMBJM di Undiksha (Universitas Pendidikan Ganesha):
-- Nomor Pendaftaran: 3242000006
-- Nama Siswa: KADEK YUNI SEDANI
-- Tanggal Lahir: 2005-11-30
-- Tahun Daftar: 2024
-- Pilihan Program Studi: Pendidikan Jasmani, Kesehatan Dan Rekreasi (S1)
-- Status Kelulusan: Lulus
-Selamat bergabung menjadi bagian dari Universitas Pendidikan Ganesha, KADEK YUNI SEDANI!</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Untuk mengecek kelulusan Seleksi Mahasiswa Baru Jalur Mandiri (SMBJM), Anda dapat mengunjungi link berikut: https://penerimaan.undiksha.ac.id/smbjm/login
-Jika Anda ingin saya membantu, silakan kirimkan Nomor Pendaftaran dan Tanggal Lahir Anda. Berikut adalah format penulisan pesan yang perlu Anda gunakan:
-- Cek Kelulusan Nomor Pendaftaran [NO_PENDAFTARAN_10_DIGIT] Tanggal Lahir [YYYY-MM-DD]
-Contoh penulisan pesan yang benar adalah:
-- Cek Kelulusan Nomor Pendaftaran 1234567890 Tanggal Lahir 2001-01-31
-Silakan kirimkan informasi tersebut jika Anda memerlukan bantuan lebih lanjut.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Anda dapat melihat KTM melalui SSO Undiksha atau dengan mengirimkan pesan yang berisi NIM (Nomor Induk Mahasiswa) yang valid. NIM yang valid dari Undiksha terdiri dari 10 digit angka. 
-Untuk mengirimkan pesan, gunakan format berikut:
-- KTM [NIM]
-Contoh penulisan pesan:
-- KTM 1234567890
-Silakan kirimkan NIM Anda untuk mendapatkan informasi lebih lanjut.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Pertanyaan tersebut tidak relevan dengan konteks kampus Universitas Pendidikan Ganesha.</t>
-  </si>
-  <si>
-    <t>Salam Harmoni🙏
-Berikut informasi Kartu Tanda Mahasiswa (KTM) Anda. 
-- NIM: 2115101014
-- Anda dapat mengunduh KTM Anda melalui tautan berikut: https://aka.undiksha.ac.id/api/ktm/generate/2115101014?token=NVNnV1dv
-Silakan klik tautan tersebut untuk mengakses KTM Anda.</t>
+    <t>Total Reference Context Vector Database</t>
   </si>
 </sst>
 </file>
@@ -541,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -559,12 +347,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <b val="0"/>
@@ -582,26 +378,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -660,6 +437,44 @@
       </font>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -674,12 +489,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DE5294B-EEB2-4C8B-A347-1013CA7914CB}" name="Table13" displayName="Table13" ref="A1:C51" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:C51" xr:uid="{CA3EBB52-0541-4D84-AA27-B220DF286A8D}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B3B35749-B31A-4D58-B0DB-CB4B8BEB47E8}" name="No" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{850681BF-3655-4370-B3FA-48A29C2D0164}" name="Question" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{FC230C4E-D812-43B5-9246-5219C076560C}" name="Ground Truth" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4DE5294B-EEB2-4C8B-A347-1013CA7914CB}" name="Table13" displayName="Table13" ref="A1:D26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D26" xr:uid="{CA3EBB52-0541-4D84-AA27-B220DF286A8D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{B3B35749-B31A-4D58-B0DB-CB4B8BEB47E8}" name="No" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{850681BF-3655-4370-B3FA-48A29C2D0164}" name="Question" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{FC230C4E-D812-43B5-9246-5219C076560C}" name="Ground Truth" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{401184D3-9332-4330-8066-E2C38256198A}" name="Total Reference Context Vector Database" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -982,43 +798,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C236C3-56F3-4E8C-AE3B-EC9AC92EE935}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="4" customWidth="1"/>
     <col min="2" max="2" width="59.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="226.5703125" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="119.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="8" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="54" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1026,32 +849,41 @@
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="D3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1059,32 +891,41 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="D8" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1092,10 +933,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1103,10 +947,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1114,447 +961,220 @@
         <v>4</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="D17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="D22" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D24" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>26</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>27</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>28</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>29</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <v>30</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>31</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
-        <v>35</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
-        <v>36</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>37</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
-        <v>38</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
-        <v>39</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
-        <v>40</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
-        <v>41</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
-        <v>42</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
-        <v>43</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
-        <v>44</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
-        <v>45</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
-        <v>47</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
-        <v>48</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
-        <v>49</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
-        <v>50</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>101</v>
+        <v>52</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>